<commit_message>
refactor: add game btn fix
</commit_message>
<xml_diff>
--- a/export/Jogos.xlsx
+++ b/export/Jogos.xlsx
@@ -45,12 +45,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F2F2F2"/>
-        <bgColor rgb="00F2F2F2"/>
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -58,26 +58,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1">
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="header_style" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -440,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,14 +446,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="52" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="164" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="6" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,12 +484,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Descrição de Zeramento</t>
+          <t>Descrição</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Tempo Jogado</t>
+          <t>Tempo</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -533,14 +531,162 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>30:00</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
+          <t>28:00</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Max Payne</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TPS (Third-Person Shooter)</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>31/01/2025</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Bom jogo, mas só é jogavel hoje com alguns poucos mods, dificuldade elevada mas não impossivel, é bem tentativa e erro.</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Max Payne 2: The Fall of Max Payne</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>TPS (Third-Person Shooter)</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>01/02/2025</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Melhorou bastante do primeiro, até hoje muito bonito, mas o jogo começa a ficar um pouco repetitivo mais ao final.</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Deponia: The Complete Journey</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Point and Click</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>18/04/2025</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>Jogo divertido mas é impossivel jogar sem um guia</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>45:50</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Kurohyō: Ryū ga Gotoku Shinshō</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Action-Adventure</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>PlayStation Portable</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr"/>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>Planejo Jogar</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>Yakuza de PSP, não tem como ser ruim.</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>